<commit_message>
chore: added matsmo cats
</commit_message>
<xml_diff>
--- a/dictionaries/outcome/1_2/1_2_yearly_rep.xlsx
+++ b/dictionaries/outcome/1_2/1_2_yearly_rep.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcarson\Documents\GIT\ds-dictionaries\dictionaries\outcome\1_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sidohaakma/Documents/Development/Visual/ds-dictionaries/dictionaries/outcome/1_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454A15CC-BD04-498A-98A7-1A3CD7AE69CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F696824-491F-0C44-B170-1C3B8C1060CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="396">
   <si>
     <t>name</t>
   </si>
@@ -1164,13 +1164,64 @@
   </si>
   <si>
     <t>Is data raw or normalised (specify normalisation method used)</t>
+  </si>
+  <si>
+    <t>matsmo_array_</t>
+  </si>
+  <si>
+    <t>450K</t>
+  </si>
+  <si>
+    <t>EPIC</t>
+  </si>
+  <si>
+    <t>matsmo_tissue_</t>
+  </si>
+  <si>
+    <t>whole blood</t>
+  </si>
+  <si>
+    <t>cord blood</t>
+  </si>
+  <si>
+    <t>placenta</t>
+  </si>
+  <si>
+    <t>matsmo_format_</t>
+  </si>
+  <si>
+    <t>RAW</t>
+  </si>
+  <si>
+    <t>BMIQ</t>
+  </si>
+  <si>
+    <t>DASEN</t>
+  </si>
+  <si>
+    <t>SQN</t>
+  </si>
+  <si>
+    <t>RCP</t>
+  </si>
+  <si>
+    <t>NOOB</t>
+  </si>
+  <si>
+    <t>CPACOR</t>
+  </si>
+  <si>
+    <t>FUNNORM</t>
+  </si>
+  <si>
+    <t>OTHER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1210,6 +1261,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1292,7 +1349,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1324,6 +1381,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1795,15 +1853,15 @@
       <selection activeCell="D141" sqref="D141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.140625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="15.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="97.85546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="29.1640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="15.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="97.83203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1872,7 +1930,7 @@
       <c r="BF1"/>
       <c r="BG1"/>
     </row>
-    <row r="2" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -1886,7 +1944,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -1898,7 +1956,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
@@ -1912,7 +1970,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -1927,7 +1985,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1942,7 +2000,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>356</v>
       </c>
@@ -1957,7 +2015,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>358</v>
       </c>
@@ -1972,7 +2030,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -1987,7 +2045,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -2002,7 +2060,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -2017,7 +2075,7 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -2032,7 +2090,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
@@ -2046,7 +2104,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>40</v>
       </c>
@@ -2060,7 +2118,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -2074,7 +2132,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>44</v>
       </c>
@@ -2088,7 +2146,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
@@ -2102,7 +2160,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
@@ -2116,7 +2174,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>50</v>
       </c>
@@ -2130,7 +2188,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>52</v>
       </c>
@@ -2144,7 +2202,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>354</v>
       </c>
@@ -2158,7 +2216,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>54</v>
       </c>
@@ -2172,7 +2230,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>56</v>
       </c>
@@ -2186,7 +2244,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>58</v>
       </c>
@@ -2200,7 +2258,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>60</v>
       </c>
@@ -2214,7 +2272,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>62</v>
       </c>
@@ -2228,7 +2286,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>64</v>
       </c>
@@ -2242,7 +2300,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>66</v>
       </c>
@@ -2256,7 +2314,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>68</v>
       </c>
@@ -2270,7 +2328,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>71</v>
       </c>
@@ -2284,7 +2342,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>73</v>
       </c>
@@ -2298,7 +2356,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>74</v>
       </c>
@@ -2312,7 +2370,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>76</v>
       </c>
@@ -2326,7 +2384,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>78</v>
       </c>
@@ -2340,7 +2398,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>80</v>
       </c>
@@ -2354,7 +2412,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>82</v>
       </c>
@@ -2368,7 +2426,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>84</v>
       </c>
@@ -2382,7 +2440,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>86</v>
       </c>
@@ -2396,7 +2454,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>89</v>
       </c>
@@ -2410,7 +2468,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>91</v>
       </c>
@@ -2424,7 +2482,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>93</v>
       </c>
@@ -2438,7 +2496,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>95</v>
       </c>
@@ -2452,7 +2510,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>97</v>
       </c>
@@ -2466,7 +2524,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>99</v>
       </c>
@@ -2480,7 +2538,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>101</v>
       </c>
@@ -2494,7 +2552,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>103</v>
       </c>
@@ -2508,7 +2566,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>105</v>
       </c>
@@ -2522,7 +2580,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>107</v>
       </c>
@@ -2536,7 +2594,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>109</v>
       </c>
@@ -2550,7 +2608,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>111</v>
       </c>
@@ -2564,7 +2622,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
         <v>113</v>
       </c>
@@ -2578,7 +2636,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>115</v>
       </c>
@@ -2592,7 +2650,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>117</v>
       </c>
@@ -2606,7 +2664,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
         <v>119</v>
       </c>
@@ -2620,7 +2678,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
         <v>121</v>
       </c>
@@ -2634,7 +2692,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
         <v>123</v>
       </c>
@@ -2648,7 +2706,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
         <v>125</v>
       </c>
@@ -2662,7 +2720,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>127</v>
       </c>
@@ -2676,7 +2734,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
         <v>129</v>
       </c>
@@ -2690,7 +2748,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
         <v>131</v>
       </c>
@@ -2704,7 +2762,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
         <v>133</v>
       </c>
@@ -2718,7 +2776,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
         <v>135</v>
       </c>
@@ -2732,7 +2790,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
         <v>137</v>
       </c>
@@ -2746,7 +2804,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
         <v>139</v>
       </c>
@@ -2760,7 +2818,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
         <v>141</v>
       </c>
@@ -2774,7 +2832,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
         <v>143</v>
       </c>
@@ -2788,7 +2846,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
         <v>145</v>
       </c>
@@ -2802,7 +2860,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
         <v>147</v>
       </c>
@@ -2816,7 +2874,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
         <v>149</v>
       </c>
@@ -2830,7 +2888,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
         <v>151</v>
       </c>
@@ -2844,7 +2902,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
         <v>153</v>
       </c>
@@ -2858,7 +2916,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
         <v>155</v>
       </c>
@@ -2872,7 +2930,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
         <v>157</v>
       </c>
@@ -2886,7 +2944,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
         <v>159</v>
       </c>
@@ -2900,7 +2958,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
         <v>161</v>
       </c>
@@ -2914,7 +2972,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
         <v>163</v>
       </c>
@@ -2928,7 +2986,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
         <v>165</v>
       </c>
@@ -2942,7 +3000,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
         <v>167</v>
       </c>
@@ -2956,7 +3014,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
         <v>169</v>
       </c>
@@ -2970,7 +3028,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
         <v>171</v>
       </c>
@@ -2984,7 +3042,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
         <v>173</v>
       </c>
@@ -2998,7 +3056,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
         <v>175</v>
       </c>
@@ -3012,7 +3070,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
         <v>177</v>
       </c>
@@ -3026,7 +3084,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
         <v>179</v>
       </c>
@@ -3040,7 +3098,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
         <v>181</v>
       </c>
@@ -3054,7 +3112,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
         <v>183</v>
       </c>
@@ -3068,7 +3126,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="11" t="s">
         <v>185</v>
       </c>
@@ -3082,7 +3140,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="11" t="s">
         <v>187</v>
       </c>
@@ -3096,7 +3154,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="11" t="s">
         <v>189</v>
       </c>
@@ -3110,7 +3168,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="11" t="s">
         <v>191</v>
       </c>
@@ -3124,7 +3182,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="11" t="s">
         <v>193</v>
       </c>
@@ -3138,7 +3196,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="11" t="s">
         <v>195</v>
       </c>
@@ -3152,7 +3210,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="11" t="s">
         <v>197</v>
       </c>
@@ -3166,7 +3224,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="11" t="s">
         <v>199</v>
       </c>
@@ -3180,7 +3238,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="11" t="s">
         <v>201</v>
       </c>
@@ -3194,7 +3252,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="11" t="s">
         <v>203</v>
       </c>
@@ -3208,7 +3266,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="11" t="s">
         <v>205</v>
       </c>
@@ -3222,7 +3280,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="11" t="s">
         <v>207</v>
       </c>
@@ -3236,7 +3294,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="11" t="s">
         <v>209</v>
       </c>
@@ -3250,7 +3308,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="11" t="s">
         <v>211</v>
       </c>
@@ -3264,7 +3322,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="11" t="s">
         <v>213</v>
       </c>
@@ -3278,7 +3336,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="11" t="s">
         <v>215</v>
       </c>
@@ -3292,7 +3350,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="11" t="s">
         <v>217</v>
       </c>
@@ -3306,7 +3364,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="11" t="s">
         <v>219</v>
       </c>
@@ -3320,7 +3378,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="11" t="s">
         <v>221</v>
       </c>
@@ -3334,7 +3392,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
         <v>223</v>
       </c>
@@ -3348,7 +3406,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
         <v>225</v>
       </c>
@@ -3362,7 +3420,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
         <v>227</v>
       </c>
@@ -3376,7 +3434,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
         <v>229</v>
       </c>
@@ -3390,7 +3448,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="13" t="s">
         <v>231</v>
       </c>
@@ -3404,7 +3462,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>303</v>
       </c>
@@ -3418,7 +3476,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>305</v>
       </c>
@@ -3432,7 +3490,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="18" t="s">
         <v>349</v>
       </c>
@@ -3446,7 +3504,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>309</v>
       </c>
@@ -3460,7 +3518,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>350</v>
       </c>
@@ -3474,7 +3532,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>351</v>
       </c>
@@ -3488,7 +3546,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>315</v>
       </c>
@@ -3502,7 +3560,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>352</v>
       </c>
@@ -3516,7 +3574,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>353</v>
       </c>
@@ -3530,7 +3588,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>321</v>
       </c>
@@ -3544,7 +3602,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>323</v>
       </c>
@@ -3558,7 +3616,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>325</v>
       </c>
@@ -3572,7 +3630,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>327</v>
       </c>
@@ -3586,7 +3644,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>329</v>
       </c>
@@ -3600,7 +3658,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>366</v>
       </c>
@@ -3614,7 +3672,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="22" t="s">
         <v>365</v>
       </c>
@@ -3628,7 +3686,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>364</v>
       </c>
@@ -3642,7 +3700,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>363</v>
       </c>
@@ -3656,7 +3714,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="22" t="s">
         <v>367</v>
       </c>
@@ -3670,7 +3728,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>362</v>
       </c>
@@ -3684,7 +3742,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="22" t="s">
         <v>361</v>
       </c>
@@ -3698,7 +3756,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="22" t="s">
         <v>368</v>
       </c>
@@ -3712,7 +3770,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>360</v>
       </c>
@@ -3726,7 +3784,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>369</v>
       </c>
@@ -3740,7 +3798,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>370</v>
       </c>
@@ -3754,7 +3812,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>371</v>
       </c>
@@ -3768,7 +3826,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>372</v>
       </c>
@@ -3782,7 +3840,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>373</v>
       </c>
@@ -3808,20 +3866,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D244"/>
+  <dimension ref="A1:D259"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A218" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A245" sqref="A245"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A228" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A253" sqref="A253"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" style="1" customWidth="1"/>
-    <col min="2" max="4" width="18.42578125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="18.5" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
@@ -3835,7 +3893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -3849,7 +3907,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -3863,7 +3921,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -3877,7 +3935,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -3891,7 +3949,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
@@ -3905,7 +3963,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -3919,7 +3977,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>32</v>
       </c>
@@ -3933,7 +3991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -3947,7 +4005,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -3961,7 +4019,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -3975,7 +4033,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>32</v>
       </c>
@@ -3989,7 +4047,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
         <v>356</v>
       </c>
@@ -4003,7 +4061,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
         <v>356</v>
       </c>
@@ -4017,7 +4075,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
         <v>358</v>
       </c>
@@ -4031,7 +4089,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>358</v>
       </c>
@@ -4045,7 +4103,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
@@ -4059,7 +4117,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>34</v>
       </c>
@@ -4073,7 +4131,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
@@ -4087,7 +4145,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>36</v>
       </c>
@@ -4101,7 +4159,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>54</v>
       </c>
@@ -4115,7 +4173,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>54</v>
       </c>
@@ -4129,7 +4187,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>56</v>
       </c>
@@ -4143,7 +4201,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>56</v>
       </c>
@@ -4157,7 +4215,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>60</v>
       </c>
@@ -4171,7 +4229,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>60</v>
       </c>
@@ -4185,7 +4243,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>62</v>
       </c>
@@ -4199,7 +4257,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>62</v>
       </c>
@@ -4213,7 +4271,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>64</v>
       </c>
@@ -4227,7 +4285,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>64</v>
       </c>
@@ -4241,7 +4299,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>66</v>
       </c>
@@ -4255,7 +4313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>66</v>
       </c>
@@ -4269,7 +4327,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>68</v>
       </c>
@@ -4283,7 +4341,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>68</v>
       </c>
@@ -4297,7 +4355,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>91</v>
       </c>
@@ -4311,7 +4369,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>91</v>
       </c>
@@ -4325,7 +4383,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>91</v>
       </c>
@@ -4339,7 +4397,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>91</v>
       </c>
@@ -4353,7 +4411,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>91</v>
       </c>
@@ -4367,7 +4425,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>91</v>
       </c>
@@ -4381,7 +4439,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>89</v>
       </c>
@@ -4395,7 +4453,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>89</v>
       </c>
@@ -4409,7 +4467,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>89</v>
       </c>
@@ -4423,7 +4481,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>89</v>
       </c>
@@ -4437,7 +4495,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>89</v>
       </c>
@@ -4451,7 +4509,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>89</v>
       </c>
@@ -4465,7 +4523,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>105</v>
       </c>
@@ -4479,7 +4537,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>105</v>
       </c>
@@ -4493,7 +4551,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>105</v>
       </c>
@@ -4507,7 +4565,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>105</v>
       </c>
@@ -4521,7 +4579,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>105</v>
       </c>
@@ -4535,7 +4593,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>105</v>
       </c>
@@ -4549,7 +4607,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>103</v>
       </c>
@@ -4563,7 +4621,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>103</v>
       </c>
@@ -4577,7 +4635,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>103</v>
       </c>
@@ -4591,7 +4649,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>103</v>
       </c>
@@ -4605,7 +4663,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>103</v>
       </c>
@@ -4619,7 +4677,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>103</v>
       </c>
@@ -4633,7 +4691,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>119</v>
       </c>
@@ -4647,7 +4705,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>119</v>
       </c>
@@ -4661,7 +4719,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>119</v>
       </c>
@@ -4675,7 +4733,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>119</v>
       </c>
@@ -4689,7 +4747,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>119</v>
       </c>
@@ -4703,7 +4761,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>119</v>
       </c>
@@ -4717,7 +4775,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>117</v>
       </c>
@@ -4731,7 +4789,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>117</v>
       </c>
@@ -4745,7 +4803,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>117</v>
       </c>
@@ -4759,7 +4817,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>117</v>
       </c>
@@ -4773,7 +4831,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>117</v>
       </c>
@@ -4787,7 +4845,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>127</v>
       </c>
@@ -4801,7 +4859,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>127</v>
       </c>
@@ -4815,7 +4873,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>131</v>
       </c>
@@ -4829,7 +4887,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>131</v>
       </c>
@@ -4843,7 +4901,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>139</v>
       </c>
@@ -4857,7 +4915,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>139</v>
       </c>
@@ -4871,7 +4929,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>139</v>
       </c>
@@ -4885,7 +4943,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>139</v>
       </c>
@@ -4899,7 +4957,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>139</v>
       </c>
@@ -4913,7 +4971,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>139</v>
       </c>
@@ -4927,7 +4985,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>137</v>
       </c>
@@ -4941,7 +4999,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>137</v>
       </c>
@@ -4955,7 +5013,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>137</v>
       </c>
@@ -4969,7 +5027,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>137</v>
       </c>
@@ -4983,7 +5041,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>137</v>
       </c>
@@ -4997,7 +5055,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>137</v>
       </c>
@@ -5011,7 +5069,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>137</v>
       </c>
@@ -5025,7 +5083,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>137</v>
       </c>
@@ -5039,7 +5097,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>147</v>
       </c>
@@ -5053,7 +5111,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>147</v>
       </c>
@@ -5067,7 +5125,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>151</v>
       </c>
@@ -5081,7 +5139,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>151</v>
       </c>
@@ -5095,7 +5153,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>159</v>
       </c>
@@ -5109,7 +5167,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>159</v>
       </c>
@@ -5123,7 +5181,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>159</v>
       </c>
@@ -5137,7 +5195,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>159</v>
       </c>
@@ -5151,7 +5209,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>159</v>
       </c>
@@ -5165,7 +5223,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>159</v>
       </c>
@@ -5179,7 +5237,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>157</v>
       </c>
@@ -5193,7 +5251,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>157</v>
       </c>
@@ -5207,7 +5265,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>157</v>
       </c>
@@ -5221,7 +5279,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>157</v>
       </c>
@@ -5235,7 +5293,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>157</v>
       </c>
@@ -5249,7 +5307,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>157</v>
       </c>
@@ -5263,7 +5321,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>157</v>
       </c>
@@ -5277,7 +5335,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>157</v>
       </c>
@@ -5291,7 +5349,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>157</v>
       </c>
@@ -5305,7 +5363,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>157</v>
       </c>
@@ -5319,7 +5377,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>157</v>
       </c>
@@ -5333,7 +5391,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>157</v>
       </c>
@@ -5347,7 +5405,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>157</v>
       </c>
@@ -5361,7 +5419,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>157</v>
       </c>
@@ -5375,7 +5433,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>175</v>
       </c>
@@ -5389,7 +5447,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>175</v>
       </c>
@@ -5403,7 +5461,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>175</v>
       </c>
@@ -5417,7 +5475,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>175</v>
       </c>
@@ -5431,7 +5489,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>175</v>
       </c>
@@ -5445,7 +5503,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>175</v>
       </c>
@@ -5459,7 +5517,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>173</v>
       </c>
@@ -5473,7 +5531,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>173</v>
       </c>
@@ -5487,7 +5545,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>173</v>
       </c>
@@ -5501,7 +5559,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>173</v>
       </c>
@@ -5515,7 +5573,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>173</v>
       </c>
@@ -5529,7 +5587,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>173</v>
       </c>
@@ -5543,7 +5601,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>173</v>
       </c>
@@ -5557,7 +5615,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>173</v>
       </c>
@@ -5571,7 +5629,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>173</v>
       </c>
@@ -5585,7 +5643,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>173</v>
       </c>
@@ -5599,7 +5657,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
         <v>173</v>
       </c>
@@ -5613,7 +5671,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>173</v>
       </c>
@@ -5627,7 +5685,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>173</v>
       </c>
@@ -5641,7 +5699,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>173</v>
       </c>
@@ -5655,7 +5713,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>173</v>
       </c>
@@ -5669,7 +5727,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>173</v>
       </c>
@@ -5683,7 +5741,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>173</v>
       </c>
@@ -5697,7 +5755,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>191</v>
       </c>
@@ -5711,7 +5769,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>191</v>
       </c>
@@ -5725,7 +5783,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>191</v>
       </c>
@@ -5739,7 +5797,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>191</v>
       </c>
@@ -5753,7 +5811,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>191</v>
       </c>
@@ -5767,7 +5825,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>191</v>
       </c>
@@ -5781,7 +5839,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>189</v>
       </c>
@@ -5795,7 +5853,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>189</v>
       </c>
@@ -5809,7 +5867,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>189</v>
       </c>
@@ -5823,7 +5881,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>189</v>
       </c>
@@ -5837,7 +5895,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>189</v>
       </c>
@@ -5851,7 +5909,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>189</v>
       </c>
@@ -5865,7 +5923,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>189</v>
       </c>
@@ -5879,7 +5937,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>189</v>
       </c>
@@ -5893,7 +5951,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>189</v>
       </c>
@@ -5907,7 +5965,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>189</v>
       </c>
@@ -5921,7 +5979,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>189</v>
       </c>
@@ -5935,7 +5993,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>189</v>
       </c>
@@ -5949,7 +6007,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
         <v>189</v>
       </c>
@@ -5963,7 +6021,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
         <v>189</v>
       </c>
@@ -5977,7 +6035,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
         <v>207</v>
       </c>
@@ -5991,7 +6049,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
         <v>207</v>
       </c>
@@ -6005,7 +6063,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="4" t="s">
         <v>207</v>
       </c>
@@ -6019,7 +6077,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="4" t="s">
         <v>207</v>
       </c>
@@ -6033,7 +6091,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="4" t="s">
         <v>207</v>
       </c>
@@ -6047,7 +6105,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
         <v>207</v>
       </c>
@@ -6061,7 +6119,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="4" t="s">
         <v>205</v>
       </c>
@@ -6075,7 +6133,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
         <v>205</v>
       </c>
@@ -6089,7 +6147,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
         <v>223</v>
       </c>
@@ -6103,7 +6161,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
         <v>223</v>
       </c>
@@ -6117,7 +6175,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="4" t="s">
         <v>223</v>
       </c>
@@ -6131,7 +6189,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="4" t="s">
         <v>223</v>
       </c>
@@ -6145,7 +6203,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="4" t="s">
         <v>223</v>
       </c>
@@ -6159,7 +6217,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
         <v>223</v>
       </c>
@@ -6173,7 +6231,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
         <v>221</v>
       </c>
@@ -6187,7 +6245,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
         <v>221</v>
       </c>
@@ -6201,7 +6259,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="4" t="s">
         <v>221</v>
       </c>
@@ -6215,7 +6273,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="4" t="s">
         <v>221</v>
       </c>
@@ -6229,7 +6287,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="4" t="s">
         <v>221</v>
       </c>
@@ -6243,7 +6301,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
         <v>221</v>
       </c>
@@ -6257,7 +6315,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="4" t="s">
         <v>221</v>
       </c>
@@ -6271,7 +6329,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
         <v>221</v>
       </c>
@@ -6285,7 +6343,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="4" t="s">
         <v>221</v>
       </c>
@@ -6299,7 +6357,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="4" t="s">
         <v>221</v>
       </c>
@@ -6313,7 +6371,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
         <v>221</v>
       </c>
@@ -6327,7 +6385,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
         <v>221</v>
       </c>
@@ -6341,7 +6399,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="181" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
         <v>221</v>
       </c>
@@ -6355,7 +6413,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="182" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
         <v>221</v>
       </c>
@@ -6369,7 +6427,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="183" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="4" t="s">
         <v>221</v>
       </c>
@@ -6383,7 +6441,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
         <v>221</v>
       </c>
@@ -6397,7 +6455,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="185" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
         <v>221</v>
       </c>
@@ -6411,7 +6469,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="4" t="s">
         <v>221</v>
       </c>
@@ -6425,7 +6483,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
         <v>221</v>
       </c>
@@ -6439,7 +6497,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="188" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
         <v>221</v>
       </c>
@@ -6453,7 +6511,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
         <v>221</v>
       </c>
@@ -6467,7 +6525,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="4" t="s">
         <v>221</v>
       </c>
@@ -6481,7 +6539,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="4" t="s">
         <v>221</v>
       </c>
@@ -6495,7 +6553,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="4" t="s">
         <v>221</v>
       </c>
@@ -6509,7 +6567,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="4" t="s">
         <v>221</v>
       </c>
@@ -6523,7 +6581,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="4" t="s">
         <v>221</v>
       </c>
@@ -6537,7 +6595,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="4" t="s">
         <v>221</v>
       </c>
@@ -6551,7 +6609,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
         <v>221</v>
       </c>
@@ -6565,7 +6623,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="4" t="s">
         <v>221</v>
       </c>
@@ -6579,7 +6637,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="10" t="s">
         <v>221</v>
       </c>
@@ -6593,7 +6651,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="16" t="s">
         <v>303</v>
       </c>
@@ -6607,7 +6665,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="16" t="s">
         <v>303</v>
       </c>
@@ -6621,7 +6679,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="16" t="s">
         <v>305</v>
       </c>
@@ -6635,7 +6693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="16" t="s">
         <v>305</v>
       </c>
@@ -6649,7 +6707,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="16" t="s">
         <v>307</v>
       </c>
@@ -6663,7 +6721,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="16" t="s">
         <v>349</v>
       </c>
@@ -6677,7 +6735,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="16" t="s">
         <v>309</v>
       </c>
@@ -6691,7 +6749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="16" t="s">
         <v>309</v>
       </c>
@@ -6705,7 +6763,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="16" t="s">
         <v>311</v>
       </c>
@@ -6719,7 +6777,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="16" t="s">
         <v>311</v>
       </c>
@@ -6733,7 +6791,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="16" t="s">
         <v>313</v>
       </c>
@@ -6747,7 +6805,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="16" t="s">
         <v>313</v>
       </c>
@@ -6761,7 +6819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="16" t="s">
         <v>315</v>
       </c>
@@ -6775,7 +6833,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="16" t="s">
         <v>315</v>
       </c>
@@ -6789,7 +6847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="16" t="s">
         <v>317</v>
       </c>
@@ -6803,7 +6861,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="16" t="s">
         <v>317</v>
       </c>
@@ -6817,7 +6875,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="16" t="s">
         <v>319</v>
       </c>
@@ -6831,7 +6889,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="16" t="s">
         <v>319</v>
       </c>
@@ -6845,7 +6903,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="16" t="s">
         <v>321</v>
       </c>
@@ -6859,7 +6917,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="16" t="s">
         <v>321</v>
       </c>
@@ -6873,7 +6931,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="16" t="s">
         <v>323</v>
       </c>
@@ -6887,7 +6945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="16" t="s">
         <v>323</v>
       </c>
@@ -6901,7 +6959,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="16" t="s">
         <v>325</v>
       </c>
@@ -6915,7 +6973,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="16" t="s">
         <v>325</v>
       </c>
@@ -6929,7 +6987,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="16" t="s">
         <v>327</v>
       </c>
@@ -6943,7 +7001,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="16" t="s">
         <v>327</v>
       </c>
@@ -6957,7 +7015,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="16" t="s">
         <v>329</v>
       </c>
@@ -6971,7 +7029,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="16" t="s">
         <v>329</v>
       </c>
@@ -6985,7 +7043,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="16" t="s">
         <v>331</v>
       </c>
@@ -6999,7 +7057,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="16" t="s">
         <v>331</v>
       </c>
@@ -7013,7 +7071,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="16" t="s">
         <v>333</v>
       </c>
@@ -7027,7 +7085,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="16" t="s">
         <v>333</v>
       </c>
@@ -7041,7 +7099,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="16" t="s">
         <v>335</v>
       </c>
@@ -7055,7 +7113,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="16" t="s">
         <v>335</v>
       </c>
@@ -7069,7 +7127,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="16" t="s">
         <v>337</v>
       </c>
@@ -7083,7 +7141,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="16" t="s">
         <v>337</v>
       </c>
@@ -7097,7 +7155,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="16" t="s">
         <v>339</v>
       </c>
@@ -7111,7 +7169,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="16" t="s">
         <v>339</v>
       </c>
@@ -7125,7 +7183,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="16" t="s">
         <v>341</v>
       </c>
@@ -7139,7 +7197,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="16" t="s">
         <v>341</v>
       </c>
@@ -7153,7 +7211,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="16" t="s">
         <v>343</v>
       </c>
@@ -7167,7 +7225,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="16" t="s">
         <v>343</v>
       </c>
@@ -7181,7 +7239,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="241" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="16" t="s">
         <v>345</v>
       </c>
@@ -7195,7 +7253,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="242" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="16" t="s">
         <v>345</v>
       </c>
@@ -7209,7 +7267,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="243" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="16" t="s">
         <v>347</v>
       </c>
@@ -7223,7 +7281,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="244" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="16" t="s">
         <v>347</v>
       </c>
@@ -7235,6 +7293,216 @@
       </c>
       <c r="D244" s="17" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A245" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="B245" s="23">
+        <v>1</v>
+      </c>
+      <c r="C245" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D245" s="23" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A246" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="B246" s="23">
+        <v>2</v>
+      </c>
+      <c r="C246" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D246" s="23" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A247" s="22" t="s">
+        <v>382</v>
+      </c>
+      <c r="B247" s="23">
+        <v>1</v>
+      </c>
+      <c r="C247" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D247" s="23" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A248" s="22" t="s">
+        <v>382</v>
+      </c>
+      <c r="B248" s="23">
+        <v>2</v>
+      </c>
+      <c r="C248" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D248" s="23" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A249" s="22" t="s">
+        <v>382</v>
+      </c>
+      <c r="B249" s="23">
+        <v>3</v>
+      </c>
+      <c r="C249" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D249" s="23" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A250" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="B250" s="23">
+        <v>0</v>
+      </c>
+      <c r="C250" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D250" s="23" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A251" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="B251" s="23">
+        <v>1</v>
+      </c>
+      <c r="C251" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D251" s="23" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A252" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="B252" s="23">
+        <v>2</v>
+      </c>
+      <c r="C252" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D252" s="23" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A253" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="B253" s="23">
+        <v>3</v>
+      </c>
+      <c r="C253" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D253" s="23" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A254" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="B254" s="23">
+        <v>4</v>
+      </c>
+      <c r="C254" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D254" s="23" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A255" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="B255" s="23">
+        <v>5</v>
+      </c>
+      <c r="C255" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D255" s="23" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A256" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="B256" s="23">
+        <v>6</v>
+      </c>
+      <c r="C256" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D256" s="23" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A257" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="B257" s="23">
+        <v>7</v>
+      </c>
+      <c r="C257" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D257" s="23" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A258" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="B258" s="23">
+        <v>8</v>
+      </c>
+      <c r="C258" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D258" s="23" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A259" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="B259" s="23">
+        <v>9</v>
+      </c>
+      <c r="C259" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D259" s="23" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>